<commit_message>
Added Matteo Mazzola team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,84 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Matteo Mazzola</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Stefano Pizzini</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Marco Gerola</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Michele Parisi</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Andrea Anzelini</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Davide Raffaelli</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Soldatino di Pb team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Soldatino di Pb</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Stefano Pizzini</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Matteo Mazzola</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Davide Raffaelli</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Michele Parisi</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Leonardo Parisi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Andrea Conzatti  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,38 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Andrea Conzatti </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Gabriel Melis | Demobusters</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Davide Deimichei | SdrumALA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Tommaso Caliari | RSA United</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Raffa prova team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Raffa prova</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Stefano Pizzini | MediaserT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MARCO HEIDEMPERGHER | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Giovanni Torboli | F.C. Gorillaz</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Nicola Lorenzi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,38 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Nicola Lorenzi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Federico  Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Leonardo  Parisi  | MediaserT</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Frasca Luca team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,38 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Frasca Luca</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>daniel pedrotti | iMontagna</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Davide Raffaelli | MediaserT</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Michele Bertolini team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Michele Bertolini</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nicola Togni | RSA United</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alessandro Fait | RSA United</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Leonardo  Parisi  | MediaserT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Luca Lasta | La Contea FC</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Emanuele Miorandi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,6 +717,38 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Emanuele Miorandi</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Samuele Kettamier | SBARX</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alessio Zandonai | SBARX</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Danny Giordani | I Magnifici</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Riccardo Zaffoni  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -749,6 +749,38 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Riccardo Zaffoni </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Riccardo Zaffoni | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Daniele Ruzzenenti | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Leonardo Parisi  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,6 +781,38 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leonardo Parisi </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Federico  Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Nicholas Marzadro | SBARX</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Maverick  Bertolini | A.C. Denti</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added NAZARENA RAOS team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -841,6 +841,38 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>NAZARENA RAOS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Daniele  Dalbosco | iMontagna</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ANDREA ASTE | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Matteo Zanlucchi | SBARX</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Federico  Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Stefano Mattioli | MAI UNA GIOIA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added LORENZA SIMONCELLI team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +873,38 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LORENZA SIMONCELLI</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Riccardo Versini | Modium</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Antonio Calabrò | Avanzi</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Matteo Diener | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Niccolò Orsi | SBARX</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ENRICO BORDIGNON | Pinguini Trentini</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Valentina Perghem  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -905,6 +905,38 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Valentina Perghem </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Alessandro Festi | La Contea FC</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Edoardo Pomarolli | Modium</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Niccolò Orsi | SBARX</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Andrea Menolli | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Federico Fasanelli team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -937,6 +937,38 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Federico Fasanelli</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Nadir Chtioui | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Mattia Festi | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Alessandro  Tengattini | Herta Vernello</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Nicholas Marzadro team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -969,6 +969,38 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Nicholas Marzadro</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Samuele Kettamier | SBARX</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Leonardo  Parisi  | MediaserT</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Mattia Festi | Shark Attack</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Luca Giordani team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1001,6 +1001,38 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Luca Giordani</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Alberto Cerisara | Shark Attack</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ALESSIO FARINATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Antonio Calabrò | Avanzi</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Leonardo Fedrigotti | Nazionale Ferrovieri</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Licia Fondriest  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1033,6 +1033,38 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Licia Fondriest </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Stefano  Galvagni | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Edoardo Pomarolli | Modium</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Luca Giordani | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Halzyd  Pupuleku | F.C. Sala Giardini</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Marco sala team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1065,6 +1065,38 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Marco sala</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>daniel pedrotti | iMontagna</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Daniele Dalbosco | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Simoncelli Matteo  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1097,6 +1097,38 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simoncelli Matteo </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Lorenzo Canali | Herta Vernello</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Nadir Chtioui | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Matteo  Simoncelli | Herta Vernello</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Andrea Riolfatti team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1129,6 +1129,38 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Andrea Riolfatti</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Maickol Azocar | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Stefano  Galvagni | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added MATTEO MARANER team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1161,6 +1161,38 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>MATTEO MARANER</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ANDREA MANFREDI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Federico  Mortillaro | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Gentian Capa | FC. Stallions</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Teschio Fiammeggiante  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1193,6 +1193,38 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Teschio Fiammeggiante </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>daniel pedrotti | iMontagna</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Gabriele Brentari | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Simone Miorelli | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added mattia spagnolli team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1225,6 +1225,38 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>mattia spagnolli</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MATTEO PILATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Simone Schonsberg | I Magnifici</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Jacopo Ricci team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1257,6 +1257,38 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Jacopo Ricci</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Daniele  Dalbosco | iMontagna</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>MARTINO TAMONI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Halzyd  Pupuleku | F.C. Sala Giardini</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Alessandro GALVAGNI team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1289,6 +1289,38 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Alessandro GALVAGNI</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Davide Raffaelli | MediaserT</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>MATTEO BRIGO | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Daniele Ruzzenenti | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Niccoló Orsi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1321,6 +1321,38 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Niccoló Orsi</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Mattia Festi | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Michael Bertè | A.C. Denti</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Alessio Zandonai team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1353,6 +1353,38 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Alessio Zandonai</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Daniele  Dalbosco | iMontagna</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Matteo Zanlucchi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1417,6 +1417,38 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Matteo Zanlucchi</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Federico  Fasanelli  | Herta Vernello</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Simone Miorelli | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Thomas Debiasi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1449,6 +1449,38 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Daniele Dalbosco | SdrumALA</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Gennaro Bullo team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1481,6 +1481,38 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Gennaro Bullo</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ENRICO BORDIGNON | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Randy Cobbinah | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Matteo Mazzola | MediaserT</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Horto Muso team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1513,6 +1513,38 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Horto Muso</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Daniele Dalbosco | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Marco sartorelli team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1545,6 +1545,38 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Marco sartorelli</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Samuele Kettamier | SBARX</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Luca Barozzi | Modium</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Maickol Azocar | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Francesco Vettori | F.C. Julia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Savignagne ✨ team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1577,6 +1577,38 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Savignagne ✨</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Stefano  Galvagni | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Matteo Mazzola | MediaserT</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Simone Miorelli | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Daniele Ruzzenenti  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1609,6 +1609,38 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniele Ruzzenenti </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Alessandro  Maffei | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Riccardo Zeni | Demobusters</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Jacopo Zecchinelli | Vigili del Fusto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Tommaso Bruschetti team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1673,6 +1673,38 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Tommaso Bruschetti</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ELIA BATTISTI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Roberto Barozzi | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Luca Perenzoni team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,6 +1705,38 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Luca Perenzoni</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Riccardo Versini | Modium</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Andrea Bertolini | Modium</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Alessio Koleci | FC. Stallions</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Davide Rosà team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1737,6 +1737,38 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Davide Rosà</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Elia Barozzi | I Magnifici</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Alberto Simoncelli | I Magnifici</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Alessio Farinati team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1769,6 +1769,38 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Alessio Farinati</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Daniele  Dalbosco | iMontagna</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>ALESSIO FARINATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>MARCO HEIDEMPERGHER | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Federico Rippa | Vigili del Fusto</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Raffaele Prezzi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1801,6 +1801,38 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Raffaele Prezzi</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Elia Barozzi | I Magnifici</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Filippo Benetti | I Magnifici</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Andreas Galli | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Carlo Pomarolli team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1833,6 +1833,38 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Carlo Pomarolli</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Thomas Debiasi | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Randy Cobbinah | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Michele Parisi  | MediaserT</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Elia Barozzi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1897,6 +1897,38 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Elia Barozzi</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Elia Barozzi | I Magnifici</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Davide Fontana | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Team Pesto nel Tigullio team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1929,6 +1929,38 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Team Pesto nel Tigullio</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>MATTEO PILATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Alessandro Comper | F.C. Gorillaz</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Michele Merighi | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Maverick  Bertolini | A.C. Denti</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Riccardo Zeni team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1993,6 +1993,38 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Riccardo Zeni</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Samuele Kettamier | SBARX</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Eduardo  Grazioli  | FC Savignano</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Nadir Chtioui | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Roberto Barozzi | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Davide Zeni  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2025,6 +2025,38 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davide Zeni </t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Alessandro  Ruele | F.C. Gorillaz</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Eduardo  Grazioli  | FC Savignano</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Andrea Menolli | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Emanuele Tomasoni  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2057,6 +2057,38 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emanuele Tomasoni </t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>MATTEO PILATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Elia Tomasoni | Demobusters</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Marco  Sartorelli | Modium</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Nicolò Speziali | F.C. Gorillaz</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Niccolò Orsi | SBARX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added T come tigro team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2089,6 +2089,38 @@
         </is>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>T come tigro</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>MATTEO PILATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Sebastiano Zoller | CGB Gamberoni</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Roberto Barozzi | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Bestie del nord  team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2121,6 +2121,38 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bestie del nord </t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>ALESSIO FARINATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Andrea Bertolini | Modium</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Matteo Bazzanella | Hellas Madonna</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Halzyd  Pupuleku | F.C. Sala Giardini</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Bazzano Davide team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2153,6 +2153,38 @@
         </is>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Bazzano Davide</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Alberto Cerisara | Shark Attack</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Andrea Conzatti | FC Savignano</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Federico Andreis | iMontagna</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Leonardo Trinco | Vigili del Fusto</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Daniele Ruzzenenti | Demobusters</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Elena Bruschetti team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2185,6 +2185,38 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Elena Bruschetti</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Nicola Togni | RSA United</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Stefano  Galvagni | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Carlo Stedile | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>ANDREA ASTE | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Daniele Feltrinelli team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2217,6 +2217,38 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Daniele Feltrinelli</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>ANDREA ASTE | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Blendi Capa | FC. Stallions</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Daniel Azzolini team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2249,6 +2249,38 @@
         </is>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Daniel Azzolini</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Marco  Sartorelli | Modium</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Feltrinelli Daniele team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2281,6 +2281,38 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Feltrinelli Daniele</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Matteo Azzolini team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2313,6 +2313,38 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Matteo Azzolini</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>MATTEO PILATI | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Mattia Baldessarini | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>ENRICO BORDIGNON | Pinguini Trentini</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Stefano  Galvagni | Clitoriders</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Davide  Bazzano  | iMontagna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Andrea Barozzi team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2345,6 +2345,38 @@
         </is>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Andrea Barozzi</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Michele Ruele | Avanzi</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Luca Frasca | Clitoriders</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Antonio Calabrò | Avanzi</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Alessandro Fait | RSA United</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Thomas Cavagna | MAI UNA GIOIA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Michele Bertolini 2 team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2377,6 +2377,38 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Michele Bertolini 2</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Leonardo Viola | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Nicholas Marzadro | SBARX</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>FEDERICO NICOLODI | U.S. Guarna</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Francesca Sartori team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,6 +2409,38 @@
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Francesca Sartori</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Elia Barozzi | I Magnifici</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Edoardo Pomarolli | Modium</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Giacomo Gasparini | MAI UNA GIOIA</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Leonardo  Parisi  | MediaserT</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Daniele Dalbosco | SdrumALA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Anna Zandonati team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2441,6 +2441,38 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Anna Zandonati</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Stefano Tita | Clitoriders</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Mattia Festi | Shark Attack</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Alessio Bragagna | FC Savignano</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Federico  Manica | iMontagna</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Alessandro  Tengattini | Herta Vernello</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: updated Tommaso Stedile team
</commit_message>
<xml_diff>
--- a/assets/2024_squadre.xlsx
+++ b/assets/2024_squadre.xlsx
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Tommaso Stedile</t>
   </si>
   <si>
-    <t xml:space="preserve">Nicolas Giordani | FC Savignano</t>
+    <t xml:space="preserve">Federico Leonardi | Sughi ebbasta</t>
   </si>
   <si>
     <t xml:space="preserve">Filippo Benetti | I Magnifici</t>
@@ -632,14 +632,14 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="33.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.42"/>

</xml_diff>